<commit_message>
EOD commit, added text cleaning to functions and archival process prior to ETL save
</commit_message>
<xml_diff>
--- a/docs/DataModel.xlsx
+++ b/docs/DataModel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\helen\Documents\Python\AncientTrees\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DB1574-F175-4591-A7EE-6F419D527161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6760E487-F14D-4F29-854F-15FADB644ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-3705" windowWidth="29040" windowHeight="15720" xr2:uid="{420490D2-F558-47FF-B634-1361EBD30455}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="105">
   <si>
     <t>Id</t>
   </si>
@@ -156,9 +156,6 @@
   </si>
   <si>
     <t>PublicAccessibilityGroup</t>
-  </si>
-  <si>
-    <t>ColumnName</t>
   </si>
   <si>
     <t>DataType</t>
@@ -404,6 +401,15 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>34 fields, &lt;100k records</t>
+  </si>
+  <si>
+    <t>3 fields, &lt;500k records</t>
+  </si>
+  <si>
+    <t>Column Name</t>
   </si>
 </sst>
 </file>
@@ -551,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -589,6 +595,9 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -605,6 +614,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -921,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD22F74-74E4-45FE-9CEB-A44F00405A28}">
-  <dimension ref="A2:T40"/>
+  <dimension ref="A2:T42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -933,12 +945,15 @@
     <col min="2" max="2" width="9.109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="28.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.21875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="5" customWidth="1"/>
     <col min="6" max="6" width="30.5546875" style="9" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" style="5" customWidth="1"/>
     <col min="8" max="8" width="24.5546875" style="5" customWidth="1"/>
     <col min="9" max="9" width="8.5546875" style="5" customWidth="1"/>
-    <col min="10" max="13" width="8.88671875" style="5"/>
+    <col min="10" max="10" width="8.88671875" style="5"/>
+    <col min="11" max="11" width="13.6640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" style="5" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" style="5" customWidth="1"/>
     <col min="14" max="14" width="38.33203125" style="5" customWidth="1"/>
     <col min="15" max="15" width="13.33203125" style="5" customWidth="1"/>
     <col min="16" max="16" width="11.88671875" style="5" customWidth="1"/>
@@ -949,25 +964,25 @@
   <sheetData>
     <row r="2" spans="1:20" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
-      <c r="B2" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
+      <c r="B2" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
+      <c r="J2" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
@@ -975,18 +990,18 @@
     </row>
     <row r="3" spans="1:20" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
-      <c r="B3" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
+      <c r="B3" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="15" t="s">
-        <v>99</v>
+      <c r="J3" s="16" t="s">
+        <v>98</v>
       </c>
       <c r="K3" s="16"/>
       <c r="L3" s="16"/>
@@ -1001,425 +1016,427 @@
     </row>
     <row r="4" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
-      <c r="B4" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="B4" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
+      <c r="J4" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
     </row>
-    <row r="5" spans="1:20" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="B5" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
+      <c r="J5" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
     </row>
-    <row r="6" spans="1:20" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
-      <c r="B6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
     </row>
-    <row r="7" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="2">
+    <row r="7" spans="1:20" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+    </row>
+    <row r="8" spans="1:20" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+    </row>
+    <row r="9" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
         <v>0</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J8" s="2">
-        <v>1</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
-        <v>2</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>47</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="J9" s="2">
+      <c r="G11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="2">
         <v>2</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
+      <c r="K11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="2">
         <v>3</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="D12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="2">
-        <v>4</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="G12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="2">
-        <v>5</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
+        <v>6</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B16" s="2">
+        <v>7</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B17" s="2">
         <v>8</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="D17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="2">
-        <v>9</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="2">
-        <v>10</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="F17" s="4" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>91</v>
@@ -1428,251 +1445,251 @@
         <v>13</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
+        <v>12</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="2">
+        <v>13</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="2">
         <v>14</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B22" s="2">
-        <v>15</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B23" s="2">
-        <v>16</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>9</v>
-      </c>
       <c r="D23" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B24" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B25" s="2">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>90</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B26" s="2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>90</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
+        <v>18</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B27" s="2">
+      <c r="F27" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B28" s="2">
+        <v>19</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B29" s="2">
         <v>20</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C29" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B28" s="2">
-        <v>21</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B29" s="2">
-        <v>22</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>20</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>91</v>
@@ -1681,102 +1698,102 @@
         <v>13</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="72" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B30" s="2">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" ht="72" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B31" s="2">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="72" x14ac:dyDescent="0.3">
       <c r="B32" s="2">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="2:9" ht="72" x14ac:dyDescent="0.3">
       <c r="B33" s="2">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H33" s="2">
         <v>0</v>
@@ -1784,22 +1801,22 @@
     </row>
     <row r="34" spans="2:9" ht="72" x14ac:dyDescent="0.3">
       <c r="B34" s="2">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H34" s="2">
         <v>0</v>
@@ -1807,22 +1824,22 @@
     </row>
     <row r="35" spans="2:9" ht="72" x14ac:dyDescent="0.3">
       <c r="B35" s="2">
+        <v>26</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="10" t="s">
-        <v>26</v>
-      </c>
       <c r="D35" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H35" s="2">
         <v>0</v>
@@ -1830,129 +1847,178 @@
     </row>
     <row r="36" spans="2:9" ht="72" x14ac:dyDescent="0.3">
       <c r="B36" s="2">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H36" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" ht="72" x14ac:dyDescent="0.3">
       <c r="B37" s="2">
+        <v>28</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="B38" s="2">
+        <v>29</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B39" s="2">
         <v>30</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C39" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="4" t="s">
+      <c r="D39" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B40" s="2">
+        <v>31</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B38" s="2">
-        <v>31</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="4" t="s">
+      <c r="G40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B41" s="2">
+        <v>32</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B39" s="2">
-        <v>32</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" s="4" t="s">
+      <c r="G41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B42" s="2">
+        <v>33</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B40" s="2">
-        <v>33</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I40" s="9"/>
+      <c r="G42" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I42" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="11">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B7:H7"/>
     <mergeCell ref="J2:P2"/>
     <mergeCell ref="J3:P3"/>
     <mergeCell ref="J4:P4"/>
+    <mergeCell ref="J7:P7"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="J6:P6"/>
     <mergeCell ref="J5:P5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>